<commit_message>
finished python script for ttest
</commit_message>
<xml_diff>
--- a/14-16.SurveyResults.xlsx
+++ b/14-16.SurveyResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\FRI\DIY\FRIome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8113BFD-0509-43FF-86EA-C63E903028FA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B69252-7071-40C2-A190-2D6891F00378}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8484" xr2:uid="{ADA08893-DF5E-4D7D-A0F3-2D9327F29C2B}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8635" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8638" uniqueCount="798">
   <si>
     <t>Male</t>
   </si>
@@ -2415,6 +2415,15 @@
   </si>
   <si>
     <t>religion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.Q2, s.Q3, s.Q4, s.Q5, s.Q6, s.Q7, s.Q9, s.Q10, s.Q11, s.Q12, s.Q13, s.Q14, s.Q15, s.Q18, s.Q21, s.Q23, s.Q24, s.Q25, s.Q26, s.Q30, s.Q33, s.Q34, s.Q35, s.Q36, s.Q37, s.Q38, s.Q39, s.Q40, s.Q41, s.Q42, s.Q45, s.Q46, s.Q47, s.Q48, s.Q49, s.Q50, s.Q51, s.Q52, s.Q54, s.Q55, s.Q56, s.Q57, s.Q58, s.Q59, s.Q60, s.Q61, s.Q62, s.Q63, s.Q64, s.Q65, s.Q66, s.Q67, s.Q68, s.Q69, s.Q70, s.Q71, s.Q72, s.Q73, s.Q75, s.Q76, s.Q77, s.Q78, s.Q79, s.Q80, s.Q81, s.Q83, s.Q86, s.Q87, s.Q88, s.Q90, s.Q94, s.Q96, s.Q97, s.Q98, s.Q99, s.Q100, s.Q103, s.Q104, s.Q105, s.Q106, s.Q107, s.Q108, s.Q109, s.Q110, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.Q2, s.Q3, s.Q4, s.Q5, s.Q6, s.Q7, s.Q9, s.Q10, s.Q11, s.Q12, s.Q13, s.Q14, s.Q15, s.Q18, s.Q21, s.Q23, s.Q24, s.Q25, s.Q26, s.Q30, s.Q33, s.Q34, s.Q35, s.Q36, s.Q37, s.Q38, s.Q39, s.Q40, s.Q41, s.Q42, s.Q45, s.Q46, s.Q47, s.Q48, s.Q49, s.Q50, s.Q51, s.Q52, s.Q54, s.Q55, s.Q56, s.Q57, s.Q58, s.Q59, s.Q60, s.Q61, s.Q62, s.Q63, s.Q64, s.Q65, s.Q66, s.Q67, s.Q68, s.Q69, s.Q70, s.Q71, s.Q72, s.Q75, s.Q76, s.Q77, s.Q78, s.Q79, s.Q80, s.Q83, s.Q86, s.Q87, s.Q88, s.Q90, s.Q94, s.Q96, s.Q97, s.Q98, s.Q99, s.Q100, s.Q103, s.Q104, s.Q105, s.Q106, s.Q107, s.Q108, s.Q109, s.Q110, </t>
   </si>
 </sst>
 </file>
@@ -2781,12 +2790,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B62CC5D-1A8E-4295-9B5E-1673A5C13676}">
-  <dimension ref="A1:DS138"/>
+  <dimension ref="A1:DS142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="CU1" sqref="CU1"/>
-      <selection pane="bottomLeft" activeCell="CF140" sqref="CF140"/>
+      <selection pane="bottomLeft" activeCell="AJ113" sqref="AJ113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -46388,33 +46397,488 @@
       </c>
     </row>
     <row r="138" spans="1:121" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>795</v>
+      </c>
+      <c r="D138" t="str">
+        <f>_xlfn.CONCAT("s.", D2, ", ")</f>
+        <v xml:space="preserve">s.Q2, </v>
+      </c>
+      <c r="E138" t="str">
+        <f t="shared" ref="E138:BP138" si="0">_xlfn.CONCAT("s.", E2, ", ")</f>
+        <v xml:space="preserve">s.Q3, </v>
+      </c>
+      <c r="F138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q4, </v>
+      </c>
+      <c r="G138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q5, </v>
+      </c>
+      <c r="H138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q6, </v>
+      </c>
+      <c r="I138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q7, </v>
+      </c>
+      <c r="J138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q8, </v>
+      </c>
+      <c r="K138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q9, </v>
+      </c>
+      <c r="L138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q10, </v>
+      </c>
+      <c r="M138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q11, </v>
+      </c>
+      <c r="N138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q12, </v>
+      </c>
+      <c r="O138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q13, </v>
+      </c>
+      <c r="P138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q14, </v>
+      </c>
+      <c r="Q138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q15, </v>
+      </c>
+      <c r="R138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q16, </v>
+      </c>
+      <c r="S138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q17, </v>
+      </c>
+      <c r="T138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q18, </v>
+      </c>
+      <c r="U138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q19, </v>
+      </c>
+      <c r="V138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q20, </v>
+      </c>
+      <c r="W138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q21, </v>
+      </c>
+      <c r="X138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q22, </v>
+      </c>
+      <c r="Y138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q23, </v>
+      </c>
+      <c r="Z138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q24, </v>
+      </c>
+      <c r="AA138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q25, </v>
+      </c>
+      <c r="AB138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q26, </v>
+      </c>
+      <c r="AC138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q27, </v>
+      </c>
+      <c r="AD138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q28, </v>
+      </c>
+      <c r="AE138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q29, </v>
+      </c>
+      <c r="AF138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q30, </v>
+      </c>
+      <c r="AG138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q31, </v>
+      </c>
+      <c r="AH138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q32, </v>
+      </c>
+      <c r="AI138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q33, </v>
+      </c>
+      <c r="AJ138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q34, </v>
+      </c>
+      <c r="AK138" t="str">
+        <f>_xlfn.CONCAT("s.", AK2, ", ")</f>
+        <v xml:space="preserve">s.Q35, </v>
+      </c>
+      <c r="AL138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q36, </v>
+      </c>
+      <c r="AM138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q37, </v>
+      </c>
+      <c r="AN138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q38, </v>
+      </c>
+      <c r="AO138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q39, </v>
+      </c>
+      <c r="AP138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q40, </v>
+      </c>
+      <c r="AQ138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q41, </v>
+      </c>
+      <c r="AR138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q42, </v>
+      </c>
+      <c r="AS138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q43, </v>
+      </c>
+      <c r="AT138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q44, </v>
+      </c>
+      <c r="AU138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q45, </v>
+      </c>
+      <c r="AV138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q46, </v>
+      </c>
+      <c r="AW138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q47, </v>
+      </c>
+      <c r="AX138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q48, </v>
+      </c>
+      <c r="AY138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q49, </v>
+      </c>
+      <c r="AZ138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q50, </v>
+      </c>
+      <c r="BA138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q51, </v>
+      </c>
+      <c r="BB138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q52, </v>
+      </c>
+      <c r="BC138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q53, </v>
+      </c>
+      <c r="BD138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q54, </v>
+      </c>
+      <c r="BE138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q55, </v>
+      </c>
+      <c r="BF138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q56, </v>
+      </c>
+      <c r="BG138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q57, </v>
+      </c>
+      <c r="BH138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q58, </v>
+      </c>
+      <c r="BI138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q59, </v>
+      </c>
+      <c r="BJ138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s., </v>
+      </c>
+      <c r="BK138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.mouthwash.frequency, </v>
+      </c>
+      <c r="BL138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q60, </v>
+      </c>
+      <c r="BM138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q61, </v>
+      </c>
+      <c r="BN138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q62, </v>
+      </c>
+      <c r="BO138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q63, </v>
+      </c>
+      <c r="BP138" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">s.Q64, </v>
+      </c>
+      <c r="BQ138" t="str">
+        <f t="shared" ref="BQ138:DJ138" si="1">_xlfn.CONCAT("s.", BQ2, ", ")</f>
+        <v xml:space="preserve">s.Q65, </v>
+      </c>
+      <c r="BR138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q66, </v>
+      </c>
+      <c r="BS138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q67, </v>
+      </c>
+      <c r="BT138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q68, </v>
+      </c>
+      <c r="BU138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q69, </v>
+      </c>
+      <c r="BV138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q70, </v>
+      </c>
+      <c r="BW138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q71, </v>
+      </c>
+      <c r="BX138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q72, </v>
+      </c>
+      <c r="BZ138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q74, </v>
+      </c>
+      <c r="CA138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q75, </v>
+      </c>
+      <c r="CB138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q76, </v>
+      </c>
+      <c r="CC138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q77, </v>
+      </c>
+      <c r="CD138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q78, </v>
+      </c>
+      <c r="CE138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q79, </v>
+      </c>
+      <c r="CF138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q80, </v>
+      </c>
+      <c r="CH138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q82, </v>
+      </c>
+      <c r="CI138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q83, </v>
+      </c>
+      <c r="CJ138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q84, </v>
+      </c>
+      <c r="CK138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q85, </v>
+      </c>
+      <c r="CL138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q86, </v>
+      </c>
+      <c r="CM138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q87, </v>
+      </c>
+      <c r="CN138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q88, </v>
+      </c>
+      <c r="CO138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q89, </v>
+      </c>
+      <c r="CP138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q90, </v>
+      </c>
+      <c r="CQ138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q91, </v>
+      </c>
+      <c r="CR138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q92, </v>
+      </c>
+      <c r="CS138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q93, </v>
+      </c>
+      <c r="CT138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q94, </v>
+      </c>
+      <c r="CU138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q95, </v>
+      </c>
+      <c r="CV138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q96, </v>
+      </c>
+      <c r="CW138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q97, </v>
+      </c>
+      <c r="CX138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q98, </v>
+      </c>
+      <c r="CY138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q99, </v>
+      </c>
+      <c r="CZ138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q100, </v>
+      </c>
+      <c r="DA138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q101, </v>
+      </c>
+      <c r="DB138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q102, </v>
+      </c>
+      <c r="DC138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q103, </v>
+      </c>
+      <c r="DD138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q104, </v>
+      </c>
+      <c r="DE138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q105, </v>
+      </c>
+      <c r="DF138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q106, </v>
+      </c>
+      <c r="DG138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q107, </v>
+      </c>
+      <c r="DH138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q108, </v>
+      </c>
+      <c r="DI138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q109, </v>
+      </c>
+      <c r="DJ138" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">s.Q110, </v>
+      </c>
       <c r="DK138">
         <f>COUNTBLANK(DK65:DK136)</f>
         <v>56</v>
       </c>
       <c r="DL138">
-        <f t="shared" ref="DL138:DQ138" si="0">COUNTBLANK(DL65:DL136)</f>
+        <f t="shared" ref="DL138:DQ138" si="2">COUNTBLANK(DL65:DL136)</f>
         <v>66</v>
       </c>
       <c r="DM138">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>71</v>
       </c>
       <c r="DN138">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="DO138">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>63</v>
       </c>
       <c r="DP138">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="DQ138">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>39</v>
+      </c>
+    </row>
+    <row r="140" spans="1:121" x14ac:dyDescent="0.3">
+      <c r="D140" t="str">
+        <f>_xlfn.CONCAT(D138,E138,F138,G138,H138,I138,K138,L138,M138,N138,O138,P138,Q138,T138,W138,Y138,Z138,AA138,AB138,AF138,AI138,AJ138,AK138,AL138,AM138,AN138,AO138,AP138,AQ138,AR138,AU138,AV138,AW138,AX138,AY138,AZ138,BA138,BB138,BD138,BE138,BF138,BG138,BH138,BI138,BL138,BM138,BN138,BO138,BP138,BQ138,BR138,BS138,BT138,BU138,BV138,BW138,BX138,BY138,CA138,CB138,CC138,CD138,CE138,CF138,CG138,CI138,CL138,CM138,CN138,CP138,CT138,CV138,CW138,CX138,CY138,CZ138,DC138,DD138,DE138,DF138,DG138,DH138,DI138,DJ138)</f>
+        <v xml:space="preserve">s.Q2, s.Q3, s.Q4, s.Q5, s.Q6, s.Q7, s.Q9, s.Q10, s.Q11, s.Q12, s.Q13, s.Q14, s.Q15, s.Q18, s.Q21, s.Q23, s.Q24, s.Q25, s.Q26, s.Q30, s.Q33, s.Q34, s.Q35, s.Q36, s.Q37, s.Q38, s.Q39, s.Q40, s.Q41, s.Q42, s.Q45, s.Q46, s.Q47, s.Q48, s.Q49, s.Q50, s.Q51, s.Q52, s.Q54, s.Q55, s.Q56, s.Q57, s.Q58, s.Q59, s.Q60, s.Q61, s.Q62, s.Q63, s.Q64, s.Q65, s.Q66, s.Q67, s.Q68, s.Q69, s.Q70, s.Q71, s.Q72, s.Q75, s.Q76, s.Q77, s.Q78, s.Q79, s.Q80, s.Q83, s.Q86, s.Q87, s.Q88, s.Q90, s.Q94, s.Q96, s.Q97, s.Q98, s.Q99, s.Q100, s.Q103, s.Q104, s.Q105, s.Q106, s.Q107, s.Q108, s.Q109, s.Q110, </v>
+      </c>
+    </row>
+    <row r="141" spans="1:121" x14ac:dyDescent="0.3">
+      <c r="D141" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="142" spans="1:121" x14ac:dyDescent="0.3">
+      <c r="D142" t="s">
+        <v>797</v>
       </c>
     </row>
   </sheetData>

</xml_diff>